<commit_message>
cambios en el padron
</commit_message>
<xml_diff>
--- a/Padron_Unificado.xlsx
+++ b/Padron_Unificado.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Usuario\Desktop\Backend\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A346DB1-8914-41EB-A2E1-004AD1CECB88}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7E37E49-4784-4540-B158-D63EB9ADD3CC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,21 +34,9 @@
     <t>CURP</t>
   </si>
   <si>
-    <t>Fecha Ingreso</t>
-  </si>
-  <si>
     <t>Plaza</t>
   </si>
   <si>
-    <t>Sueldo Base</t>
-  </si>
-  <si>
-    <t>Aportación ISSSTEESIN</t>
-  </si>
-  <si>
-    <t>Aportación Vivienda</t>
-  </si>
-  <si>
     <t>Municipio</t>
   </si>
   <si>
@@ -284,6 +272,18 @@
   </si>
   <si>
     <t>Sueldo_Neto_Quincenal</t>
+  </si>
+  <si>
+    <t>Fecha_Ingreso</t>
+  </si>
+  <si>
+    <t>Sueldo_Base</t>
+  </si>
+  <si>
+    <t>Aportación_ISSSTEESIN</t>
+  </si>
+  <si>
+    <t>Aportación_Vivienda</t>
   </si>
 </sst>
 </file>
@@ -687,9 +687,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:O20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H1" sqref="H1"/>
+      <selection pane="bottomLeft" activeCell="K18" sqref="K18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" zeroHeight="1" x14ac:dyDescent="0.3"/>
@@ -717,7 +717,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="C1" s="4" t="s">
         <v>1</v>
@@ -729,57 +729,57 @@
         <v>3</v>
       </c>
       <c r="F1" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="G1" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="4" t="s">
-        <v>5</v>
-      </c>
       <c r="H1" s="7" t="s">
+        <v>83</v>
+      </c>
+      <c r="I1" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="J1" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="K1" s="4" t="s">
         <v>87</v>
       </c>
-      <c r="I1" s="4" t="s">
+      <c r="L1" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="M1" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="J1" s="4" t="s">
+      <c r="N1" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="K1" s="4" t="s">
+      <c r="O1" s="4" t="s">
         <v>8</v>
-      </c>
-      <c r="L1" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="M1" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="N1" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="O1" s="4" t="s">
-        <v>12</v>
       </c>
     </row>
     <row r="2" spans="1:15" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E2" t="s">
         <v>13</v>
-      </c>
-      <c r="B2" t="s">
-        <v>14</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="D2" t="s">
-        <v>16</v>
-      </c>
-      <c r="E2" t="s">
-        <v>17</v>
       </c>
       <c r="F2" s="3">
         <v>32752</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="H2" s="2">
         <v>22125.8</v>
@@ -794,10 +794,10 @@
         <v>819.11</v>
       </c>
       <c r="L2" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="M2" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="N2" s="2">
         <v>5</v>
@@ -808,25 +808,25 @@
     </row>
     <row r="3" spans="1:15" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="B3" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="D3" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="E3" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="F3" s="3">
         <v>32752</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="H3" s="2">
         <v>7170.53</v>
@@ -841,10 +841,10 @@
         <v>227.1</v>
       </c>
       <c r="L3" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="M3" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="N3" s="2">
         <v>5</v>
@@ -855,25 +855,25 @@
     </row>
     <row r="4" spans="1:15" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
+        <v>23</v>
+      </c>
+      <c r="B4" t="s">
+        <v>24</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="D4" t="s">
+        <v>26</v>
+      </c>
+      <c r="E4" t="s">
         <v>27</v>
-      </c>
-      <c r="B4" t="s">
-        <v>28</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="D4" t="s">
-        <v>30</v>
-      </c>
-      <c r="E4" t="s">
-        <v>31</v>
       </c>
       <c r="F4" s="3">
         <v>31425</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="H4" s="2">
         <v>9598.31</v>
@@ -888,10 +888,10 @@
         <v>389.02</v>
       </c>
       <c r="L4" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="M4" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="N4" s="2">
         <v>5</v>
@@ -902,25 +902,25 @@
     </row>
     <row r="5" spans="1:15" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="B5" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="D5" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="E5" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="F5" s="3">
         <v>32767</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="H5" s="2">
         <v>7784.81</v>
@@ -935,10 +935,10 @@
         <v>319.77</v>
       </c>
       <c r="L5" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="M5" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="N5" s="2">
         <v>5</v>
@@ -949,25 +949,25 @@
     </row>
     <row r="6" spans="1:15" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="B6" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="D6" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="E6" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="F6" s="3">
         <v>32087</v>
       </c>
       <c r="G6" s="2" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="H6" s="2">
         <v>7580.28</v>
@@ -982,10 +982,10 @@
         <v>227.1</v>
       </c>
       <c r="L6" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="M6" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="N6" s="2">
         <v>5</v>
@@ -996,25 +996,25 @@
     </row>
     <row r="7" spans="1:15" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="B7" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="D7" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="E7" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="F7" s="3">
         <v>32120</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="H7" s="2">
         <v>16024.4</v>
@@ -1029,10 +1029,10 @@
         <v>809.7</v>
       </c>
       <c r="L7" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="M7" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="N7" s="2">
         <v>5</v>
@@ -1043,25 +1043,25 @@
     </row>
     <row r="8" spans="1:15" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="B8" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="D8" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="E8" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="F8" s="3">
         <v>32630</v>
       </c>
       <c r="G8" s="2" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="H8" s="2">
         <v>1002.3</v>
@@ -1076,10 +1076,10 @@
         <v>30.09</v>
       </c>
       <c r="L8" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="M8" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="N8" s="2">
         <v>5</v>
@@ -1090,25 +1090,25 @@
     </row>
     <row r="9" spans="1:15" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="B9" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="D9" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="E9" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="F9" s="3">
         <v>32630</v>
       </c>
       <c r="G9" s="2" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="H9" s="2">
         <v>1002.32</v>
@@ -1123,10 +1123,10 @@
         <v>30.09</v>
       </c>
       <c r="L9" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="M9" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="N9" s="2">
         <v>5</v>
@@ -1137,25 +1137,25 @@
     </row>
     <row r="10" spans="1:15" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="B10" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="D10" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="E10" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="F10" s="3">
         <v>32630</v>
       </c>
       <c r="G10" s="2" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="H10" s="2">
         <v>990.69</v>
@@ -1170,10 +1170,10 @@
         <v>45.13</v>
       </c>
       <c r="L10" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="M10" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="N10" s="2">
         <v>5</v>
@@ -1184,25 +1184,25 @@
     </row>
     <row r="11" spans="1:15" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="B11" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="D11" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="E11" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="F11" s="3">
         <v>32630</v>
       </c>
       <c r="G11" s="2" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="H11" s="2">
         <v>2972.12</v>
@@ -1217,10 +1217,10 @@
         <v>135.38999999999999</v>
       </c>
       <c r="L11" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="M11" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="N11" s="2">
         <v>5</v>
@@ -1231,25 +1231,25 @@
     </row>
     <row r="12" spans="1:15" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="B12" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="D12" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="E12" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="F12" s="3">
         <v>32630</v>
       </c>
       <c r="G12" s="2" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="H12" s="2">
         <v>13005.6</v>
@@ -1264,10 +1264,10 @@
         <v>391.13</v>
       </c>
       <c r="L12" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="M12" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="N12" s="2">
         <v>5</v>
@@ -1278,25 +1278,25 @@
     </row>
     <row r="13" spans="1:15" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="B13" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="D13" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="E13" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="F13" s="3">
         <v>32752</v>
       </c>
       <c r="G13" s="2" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="H13" s="2">
         <v>3379.51</v>
@@ -1311,10 +1311,10 @@
         <v>175.52</v>
       </c>
       <c r="L13" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="M13" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="N13" s="2">
         <v>5</v>
@@ -1325,25 +1325,25 @@
     </row>
     <row r="14" spans="1:15" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="B14" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="D14" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="E14" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="F14" s="3">
         <v>32752</v>
       </c>
       <c r="G14" s="2" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="H14" s="2">
         <v>281.76</v>
@@ -1358,10 +1358,10 @@
         <v>16.27</v>
       </c>
       <c r="L14" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="M14" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="N14" s="2">
         <v>5</v>
@@ -1372,25 +1372,25 @@
     </row>
     <row r="15" spans="1:15" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="B15" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="D15" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="E15" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="F15" s="3">
         <v>32752</v>
       </c>
       <c r="G15" s="2" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="H15" s="2">
         <v>3379.51</v>
@@ -1405,10 +1405,10 @@
         <v>175.52</v>
       </c>
       <c r="L15" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="M15" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="N15" s="2">
         <v>5</v>
@@ -1419,25 +1419,25 @@
     </row>
     <row r="16" spans="1:15" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="B16" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="D16" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="E16" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="F16" s="3">
         <v>32752</v>
       </c>
       <c r="G16" s="2" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="H16" s="2">
         <v>1877.51</v>
@@ -1452,10 +1452,10 @@
         <v>97.51</v>
       </c>
       <c r="L16" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="M16" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="N16" s="2">
         <v>5</v>
@@ -1466,25 +1466,25 @@
     </row>
     <row r="17" spans="1:15" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="B17" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="D17" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="E17" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="F17" s="3">
         <v>32752</v>
       </c>
       <c r="G17" s="2" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="H17" s="2">
         <v>375.51</v>
@@ -1499,10 +1499,10 @@
         <v>19.5</v>
       </c>
       <c r="L17" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="M17" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="N17" s="2">
         <v>5</v>
@@ -1513,25 +1513,25 @@
     </row>
     <row r="18" spans="1:15" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="B18" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="D18" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="E18" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="F18" s="3">
         <v>32801</v>
       </c>
       <c r="G18" s="2" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="H18" s="2">
         <v>5059.53</v>
@@ -1546,10 +1546,10 @@
         <v>180.52</v>
       </c>
       <c r="L18" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="M18" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="N18" s="2">
         <v>5</v>
@@ -1560,25 +1560,25 @@
     </row>
     <row r="19" spans="1:15" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="B19" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="D19" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="E19" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="F19" s="3">
         <v>32752</v>
       </c>
       <c r="G19" s="2" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="H19" s="2">
         <v>7045.46</v>
@@ -1593,10 +1593,10 @@
         <v>227.1</v>
       </c>
       <c r="L19" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="M19" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="N19" s="2">
         <v>5</v>
@@ -1607,25 +1607,25 @@
     </row>
     <row r="20" spans="1:15" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="B20" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="D20" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="E20" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="F20" s="3">
         <v>32776</v>
       </c>
       <c r="G20" s="2" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="H20" s="2">
         <v>7000.51</v>
@@ -1640,10 +1640,10 @@
         <v>252.34</v>
       </c>
       <c r="L20" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="M20" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="N20" s="2">
         <v>5</v>

</xml_diff>

<commit_message>
cambio en el padron
</commit_message>
<xml_diff>
--- a/Padron_Unificado.xlsx
+++ b/Padron_Unificado.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Usuario\Desktop\Backend\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7E37E49-4784-4540-B158-D63EB9ADD3CC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9D4AF7A-B837-45E1-B18B-04B353BE1E09}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="167" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="391" uniqueCount="173">
   <si>
     <t>Numemp</t>
   </si>
@@ -284,15 +284,267 @@
   </si>
   <si>
     <t>Aportación_Vivienda</t>
+  </si>
+  <si>
+    <t>10121</t>
+  </si>
+  <si>
+    <t>SALAS SOLANO IRMA VERONICA</t>
+  </si>
+  <si>
+    <t>SASI700226RI7</t>
+  </si>
+  <si>
+    <t>SASI700226MSLLLR02</t>
+  </si>
+  <si>
+    <t>9334</t>
+  </si>
+  <si>
+    <t>10131</t>
+  </si>
+  <si>
+    <t>VELARDE SANCHEZ RAMONA JAQUELINE</t>
+  </si>
+  <si>
+    <t>VESR691116SJ9</t>
+  </si>
+  <si>
+    <t>VESR691116MSLLNM06</t>
+  </si>
+  <si>
+    <t>17247</t>
+  </si>
+  <si>
+    <t>10150</t>
+  </si>
+  <si>
+    <t>OLIVAS PEREZ ADELIO</t>
+  </si>
+  <si>
+    <t>OIPA611010EN0</t>
+  </si>
+  <si>
+    <t>OIPA611010HSLLRD08</t>
+  </si>
+  <si>
+    <t>8481</t>
+  </si>
+  <si>
+    <t>10160</t>
+  </si>
+  <si>
+    <t>ROJO LOPEZ MARGARITA</t>
+  </si>
+  <si>
+    <t>ROLM690802S53</t>
+  </si>
+  <si>
+    <t>ROLM690802MSLJPR00</t>
+  </si>
+  <si>
+    <t>16475</t>
+  </si>
+  <si>
+    <t>19069</t>
+  </si>
+  <si>
+    <t>24056</t>
+  </si>
+  <si>
+    <t>26872</t>
+  </si>
+  <si>
+    <t>2930</t>
+  </si>
+  <si>
+    <t>ANGOSTURA</t>
+  </si>
+  <si>
+    <t>BANORTE</t>
+  </si>
+  <si>
+    <t>29333</t>
+  </si>
+  <si>
+    <t>30047</t>
+  </si>
+  <si>
+    <t>33678</t>
+  </si>
+  <si>
+    <t>10165</t>
+  </si>
+  <si>
+    <t>ZAMUDIO AGUIRRE LOURDES ALICIA</t>
+  </si>
+  <si>
+    <t>ZAAL680320EA6</t>
+  </si>
+  <si>
+    <t>ZAAL680320MSLMGR03</t>
+  </si>
+  <si>
+    <t>29870</t>
+  </si>
+  <si>
+    <t>10175</t>
+  </si>
+  <si>
+    <t>CORRAL VALENZUELA LAZARO</t>
+  </si>
+  <si>
+    <t>COVL610810E61</t>
+  </si>
+  <si>
+    <t>COVL610810HSRRLZ08</t>
+  </si>
+  <si>
+    <t>5980</t>
+  </si>
+  <si>
+    <t>10206</t>
+  </si>
+  <si>
+    <t>JIMENEZ SANCHEZ SANTA ELISA</t>
+  </si>
+  <si>
+    <t>JISS6504151Z8</t>
+  </si>
+  <si>
+    <t>JISS650415MSLMNN09</t>
+  </si>
+  <si>
+    <t>11887</t>
+  </si>
+  <si>
+    <t>GUASAVE</t>
+  </si>
+  <si>
+    <t>12393</t>
+  </si>
+  <si>
+    <t>19256</t>
+  </si>
+  <si>
+    <t>27610</t>
+  </si>
+  <si>
+    <t>27676</t>
+  </si>
+  <si>
+    <t>28091</t>
+  </si>
+  <si>
+    <t>29257</t>
+  </si>
+  <si>
+    <t>10225</t>
+  </si>
+  <si>
+    <t>ESPINOZA ORTIZ YAMEL</t>
+  </si>
+  <si>
+    <t>EIOY710207HB3</t>
+  </si>
+  <si>
+    <t>EIOY710207MSLSRM03</t>
+  </si>
+  <si>
+    <t>10889</t>
+  </si>
+  <si>
+    <t>30802</t>
+  </si>
+  <si>
+    <t>35467</t>
+  </si>
+  <si>
+    <t>10228</t>
+  </si>
+  <si>
+    <t>URIAS BURGOS FELIPE DE JESUS</t>
+  </si>
+  <si>
+    <t>UIBF690807AM0</t>
+  </si>
+  <si>
+    <t>UIBF690807HSLRRL03</t>
+  </si>
+  <si>
+    <t>39203</t>
+  </si>
+  <si>
+    <t>10234</t>
+  </si>
+  <si>
+    <t>RIOS HEREDIA EDGAR ARTURO</t>
+  </si>
+  <si>
+    <t>RIHE710816KY3</t>
+  </si>
+  <si>
+    <t>RIHE710816HSLSRD04</t>
+  </si>
+  <si>
+    <t>42531</t>
+  </si>
+  <si>
+    <t>10247</t>
+  </si>
+  <si>
+    <t>LOPEZ BOJORQUEZ SALVADOR</t>
+  </si>
+  <si>
+    <t>LOBS641124QS6</t>
+  </si>
+  <si>
+    <t>LOBS641124HSLPJL07</t>
+  </si>
+  <si>
+    <t>2108</t>
+  </si>
+  <si>
+    <t>SINALOA</t>
+  </si>
+  <si>
+    <t>10262</t>
+  </si>
+  <si>
+    <t>LEON CARRISOZA BLANCA ZULEMA</t>
+  </si>
+  <si>
+    <t>LECB7006014K9</t>
+  </si>
+  <si>
+    <t>LECB700601MSLNRL09</t>
+  </si>
+  <si>
+    <t>14113</t>
+  </si>
+  <si>
+    <t>10268</t>
+  </si>
+  <si>
+    <t>LOPEZ CAMACHO CLAUDIO</t>
+  </si>
+  <si>
+    <t>LOCC6606203Y4</t>
+  </si>
+  <si>
+    <t>LOCC660620HSLPML01</t>
+  </si>
+  <si>
+    <t>29873</t>
+  </si>
+  <si>
+    <t>MOCORITO</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd\ hh:mm:ss"/>
-  </numFmts>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -362,15 +614,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -382,6 +631,12 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -685,77 +940,77 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:O20"/>
+  <dimension ref="A1:O48"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K18" sqref="K18"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" zeroHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="8.88671875" style="5"/>
-    <col min="2" max="2" width="41.6640625" style="5" customWidth="1"/>
-    <col min="3" max="3" width="8.88671875" style="6"/>
-    <col min="4" max="4" width="18.33203125" style="5" customWidth="1"/>
-    <col min="5" max="5" width="23.21875" style="5" customWidth="1"/>
-    <col min="6" max="6" width="25.5546875" style="6" customWidth="1"/>
-    <col min="7" max="7" width="9.77734375" style="6" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="21.109375" style="6" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="13.5546875" style="6" customWidth="1"/>
-    <col min="10" max="10" width="22" style="6" customWidth="1"/>
-    <col min="11" max="11" width="19.5546875" style="6" customWidth="1"/>
-    <col min="12" max="12" width="24" style="5" customWidth="1"/>
-    <col min="13" max="13" width="14.21875" style="5" customWidth="1"/>
-    <col min="14" max="14" width="20.5546875" style="6" customWidth="1"/>
-    <col min="15" max="15" width="8.88671875" style="6"/>
-    <col min="16" max="16384" width="8.88671875" style="5"/>
+    <col min="1" max="1" width="8.88671875" style="4"/>
+    <col min="2" max="2" width="41.6640625" style="4" customWidth="1"/>
+    <col min="3" max="3" width="8.88671875" style="5"/>
+    <col min="4" max="4" width="18.33203125" style="4" customWidth="1"/>
+    <col min="5" max="5" width="23.21875" style="4" customWidth="1"/>
+    <col min="6" max="6" width="25.5546875" style="8" customWidth="1"/>
+    <col min="7" max="7" width="9.77734375" style="5" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="21.109375" style="5" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.5546875" style="5" customWidth="1"/>
+    <col min="10" max="10" width="22" style="5" customWidth="1"/>
+    <col min="11" max="11" width="19.5546875" style="5" customWidth="1"/>
+    <col min="12" max="12" width="24" style="4" customWidth="1"/>
+    <col min="13" max="13" width="14.21875" style="4" customWidth="1"/>
+    <col min="14" max="14" width="20.5546875" style="5" customWidth="1"/>
+    <col min="15" max="15" width="8.88671875" style="5"/>
+    <col min="16" max="16384" width="8.88671875" style="4"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:15" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="B1" s="3" t="s">
         <v>82</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="C1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="D1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="E1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="F1" s="3" t="s">
         <v>84</v>
       </c>
-      <c r="G1" s="4" t="s">
+      <c r="G1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="H1" s="7" t="s">
+      <c r="H1" s="6" t="s">
         <v>83</v>
       </c>
-      <c r="I1" s="4" t="s">
+      <c r="I1" s="3" t="s">
         <v>85</v>
       </c>
-      <c r="J1" s="4" t="s">
+      <c r="J1" s="3" t="s">
         <v>86</v>
       </c>
-      <c r="K1" s="4" t="s">
+      <c r="K1" s="3" t="s">
         <v>87</v>
       </c>
-      <c r="L1" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="M1" s="4" t="s">
+      <c r="L1" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="M1" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="N1" s="4" t="s">
+      <c r="N1" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="O1" s="4" t="s">
+      <c r="O1" s="3" t="s">
         <v>8</v>
       </c>
     </row>
@@ -775,7 +1030,7 @@
       <c r="E2" t="s">
         <v>13</v>
       </c>
-      <c r="F2" s="3">
+      <c r="F2" s="7">
         <v>32752</v>
       </c>
       <c r="G2" s="2" t="s">
@@ -822,7 +1077,7 @@
       <c r="E3" t="s">
         <v>20</v>
       </c>
-      <c r="F3" s="3">
+      <c r="F3" s="7">
         <v>32752</v>
       </c>
       <c r="G3" s="2" t="s">
@@ -869,7 +1124,7 @@
       <c r="E4" t="s">
         <v>27</v>
       </c>
-      <c r="F4" s="3">
+      <c r="F4" s="7">
         <v>31425</v>
       </c>
       <c r="G4" s="2" t="s">
@@ -916,7 +1171,7 @@
       <c r="E5" t="s">
         <v>34</v>
       </c>
-      <c r="F5" s="3">
+      <c r="F5" s="7">
         <v>32767</v>
       </c>
       <c r="G5" s="2" t="s">
@@ -963,7 +1218,7 @@
       <c r="E6" t="s">
         <v>40</v>
       </c>
-      <c r="F6" s="3">
+      <c r="F6" s="7">
         <v>32087</v>
       </c>
       <c r="G6" s="2" t="s">
@@ -1010,7 +1265,7 @@
       <c r="E7" t="s">
         <v>45</v>
       </c>
-      <c r="F7" s="3">
+      <c r="F7" s="7">
         <v>32120</v>
       </c>
       <c r="G7" s="2" t="s">
@@ -1057,7 +1312,7 @@
       <c r="E8" t="s">
         <v>50</v>
       </c>
-      <c r="F8" s="3">
+      <c r="F8" s="7">
         <v>32630</v>
       </c>
       <c r="G8" s="2" t="s">
@@ -1104,7 +1359,7 @@
       <c r="E9" t="s">
         <v>50</v>
       </c>
-      <c r="F9" s="3">
+      <c r="F9" s="7">
         <v>32630</v>
       </c>
       <c r="G9" s="2" t="s">
@@ -1151,7 +1406,7 @@
       <c r="E10" t="s">
         <v>50</v>
       </c>
-      <c r="F10" s="3">
+      <c r="F10" s="7">
         <v>32630</v>
       </c>
       <c r="G10" s="2" t="s">
@@ -1198,7 +1453,7 @@
       <c r="E11" t="s">
         <v>50</v>
       </c>
-      <c r="F11" s="3">
+      <c r="F11" s="7">
         <v>32630</v>
       </c>
       <c r="G11" s="2" t="s">
@@ -1245,7 +1500,7 @@
       <c r="E12" t="s">
         <v>50</v>
       </c>
-      <c r="F12" s="3">
+      <c r="F12" s="7">
         <v>32630</v>
       </c>
       <c r="G12" s="2" t="s">
@@ -1292,7 +1547,7 @@
       <c r="E13" t="s">
         <v>59</v>
       </c>
-      <c r="F13" s="3">
+      <c r="F13" s="7">
         <v>32752</v>
       </c>
       <c r="G13" s="2" t="s">
@@ -1339,7 +1594,7 @@
       <c r="E14" t="s">
         <v>59</v>
       </c>
-      <c r="F14" s="3">
+      <c r="F14" s="7">
         <v>32752</v>
       </c>
       <c r="G14" s="2" t="s">
@@ -1386,7 +1641,7 @@
       <c r="E15" t="s">
         <v>59</v>
       </c>
-      <c r="F15" s="3">
+      <c r="F15" s="7">
         <v>32752</v>
       </c>
       <c r="G15" s="2" t="s">
@@ -1433,7 +1688,7 @@
       <c r="E16" t="s">
         <v>59</v>
       </c>
-      <c r="F16" s="3">
+      <c r="F16" s="7">
         <v>32752</v>
       </c>
       <c r="G16" s="2" t="s">
@@ -1480,7 +1735,7 @@
       <c r="E17" t="s">
         <v>59</v>
       </c>
-      <c r="F17" s="3">
+      <c r="F17" s="7">
         <v>32752</v>
       </c>
       <c r="G17" s="2" t="s">
@@ -1527,7 +1782,7 @@
       <c r="E18" t="s">
         <v>69</v>
       </c>
-      <c r="F18" s="3">
+      <c r="F18" s="7">
         <v>32801</v>
       </c>
       <c r="G18" s="2" t="s">
@@ -1574,7 +1829,7 @@
       <c r="E19" t="s">
         <v>75</v>
       </c>
-      <c r="F19" s="3">
+      <c r="F19" s="7">
         <v>32752</v>
       </c>
       <c r="G19" s="2" t="s">
@@ -1621,7 +1876,7 @@
       <c r="E20" t="s">
         <v>80</v>
       </c>
-      <c r="F20" s="3">
+      <c r="F20" s="7">
         <v>32776</v>
       </c>
       <c r="G20" s="2" t="s">
@@ -1649,6 +1904,1322 @@
         <v>5</v>
       </c>
       <c r="O20" s="2">
+        <v>2025</v>
+      </c>
+    </row>
+    <row r="21" spans="1:15" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>88</v>
+      </c>
+      <c r="B21" t="s">
+        <v>89</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D21" t="s">
+        <v>90</v>
+      </c>
+      <c r="E21" t="s">
+        <v>91</v>
+      </c>
+      <c r="F21" s="7">
+        <v>32759</v>
+      </c>
+      <c r="G21" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="H21" s="2">
+        <v>7045.51</v>
+      </c>
+      <c r="I21" s="2">
+        <v>4542.0200000000004</v>
+      </c>
+      <c r="J21" s="2">
+        <v>587.78</v>
+      </c>
+      <c r="K21" s="2">
+        <v>227.1</v>
+      </c>
+      <c r="L21" t="s">
+        <v>36</v>
+      </c>
+      <c r="M21" t="s">
+        <v>30</v>
+      </c>
+      <c r="N21" s="2">
+        <v>5</v>
+      </c>
+      <c r="O21" s="2">
+        <v>2025</v>
+      </c>
+    </row>
+    <row r="22" spans="1:15" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
+        <v>93</v>
+      </c>
+      <c r="B22" t="s">
+        <v>94</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D22" t="s">
+        <v>95</v>
+      </c>
+      <c r="E22" t="s">
+        <v>96</v>
+      </c>
+      <c r="F22" s="7">
+        <v>32764</v>
+      </c>
+      <c r="G22" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="H22" s="2">
+        <v>4269.04</v>
+      </c>
+      <c r="I22" s="2">
+        <v>3069.42</v>
+      </c>
+      <c r="J22" s="2">
+        <v>407.26</v>
+      </c>
+      <c r="K22" s="2">
+        <v>153.47</v>
+      </c>
+      <c r="L22" t="s">
+        <v>36</v>
+      </c>
+      <c r="M22" t="s">
+        <v>30</v>
+      </c>
+      <c r="N22" s="2">
+        <v>5</v>
+      </c>
+      <c r="O22" s="2">
+        <v>2025</v>
+      </c>
+    </row>
+    <row r="23" spans="1:15" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
+        <v>98</v>
+      </c>
+      <c r="B23" t="s">
+        <v>99</v>
+      </c>
+      <c r="C23" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="D23" t="s">
+        <v>100</v>
+      </c>
+      <c r="E23" t="s">
+        <v>101</v>
+      </c>
+      <c r="F23" s="7">
+        <v>32771</v>
+      </c>
+      <c r="G23" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="H23" s="2">
+        <v>7169.74</v>
+      </c>
+      <c r="I23" s="2">
+        <v>4542.0200000000004</v>
+      </c>
+      <c r="J23" s="2">
+        <v>587.78</v>
+      </c>
+      <c r="K23" s="2">
+        <v>227.1</v>
+      </c>
+      <c r="L23" t="s">
+        <v>36</v>
+      </c>
+      <c r="M23" t="s">
+        <v>16</v>
+      </c>
+      <c r="N23" s="2">
+        <v>5</v>
+      </c>
+      <c r="O23" s="2">
+        <v>2025</v>
+      </c>
+    </row>
+    <row r="24" spans="1:15" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
+        <v>103</v>
+      </c>
+      <c r="B24" t="s">
+        <v>104</v>
+      </c>
+      <c r="C24" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D24" t="s">
+        <v>105</v>
+      </c>
+      <c r="E24" t="s">
+        <v>106</v>
+      </c>
+      <c r="F24" s="7">
+        <v>32524</v>
+      </c>
+      <c r="G24" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="H24" s="2">
+        <v>1084.94</v>
+      </c>
+      <c r="I24" s="2">
+        <v>902.61</v>
+      </c>
+      <c r="J24" s="2">
+        <v>119.53</v>
+      </c>
+      <c r="K24" s="2">
+        <v>45.13</v>
+      </c>
+      <c r="L24" t="s">
+        <v>29</v>
+      </c>
+      <c r="M24" t="s">
+        <v>16</v>
+      </c>
+      <c r="N24" s="2">
+        <v>5</v>
+      </c>
+      <c r="O24" s="2">
+        <v>2025</v>
+      </c>
+    </row>
+    <row r="25" spans="1:15" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
+        <v>103</v>
+      </c>
+      <c r="B25" t="s">
+        <v>104</v>
+      </c>
+      <c r="C25" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D25" t="s">
+        <v>105</v>
+      </c>
+      <c r="E25" t="s">
+        <v>106</v>
+      </c>
+      <c r="F25" s="7">
+        <v>32524</v>
+      </c>
+      <c r="G25" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="H25" s="2">
+        <v>2134.91</v>
+      </c>
+      <c r="I25" s="2">
+        <v>1805.22</v>
+      </c>
+      <c r="J25" s="2">
+        <v>239.06</v>
+      </c>
+      <c r="K25" s="2">
+        <v>90.26</v>
+      </c>
+      <c r="L25" t="s">
+        <v>29</v>
+      </c>
+      <c r="M25" t="s">
+        <v>16</v>
+      </c>
+      <c r="N25" s="2">
+        <v>5</v>
+      </c>
+      <c r="O25" s="2">
+        <v>2025</v>
+      </c>
+    </row>
+    <row r="26" spans="1:15" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A26" t="s">
+        <v>103</v>
+      </c>
+      <c r="B26" t="s">
+        <v>104</v>
+      </c>
+      <c r="C26" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D26" t="s">
+        <v>105</v>
+      </c>
+      <c r="E26" t="s">
+        <v>106</v>
+      </c>
+      <c r="F26" s="7">
+        <v>32524</v>
+      </c>
+      <c r="G26" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="H26" s="2">
+        <v>1084.94</v>
+      </c>
+      <c r="I26" s="2">
+        <v>902.61</v>
+      </c>
+      <c r="J26" s="2">
+        <v>119.53</v>
+      </c>
+      <c r="K26" s="2">
+        <v>45.13</v>
+      </c>
+      <c r="L26" t="s">
+        <v>29</v>
+      </c>
+      <c r="M26" t="s">
+        <v>16</v>
+      </c>
+      <c r="N26" s="2">
+        <v>5</v>
+      </c>
+      <c r="O26" s="2">
+        <v>2025</v>
+      </c>
+    </row>
+    <row r="27" spans="1:15" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A27" t="s">
+        <v>103</v>
+      </c>
+      <c r="B27" t="s">
+        <v>104</v>
+      </c>
+      <c r="C27" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D27" t="s">
+        <v>105</v>
+      </c>
+      <c r="E27" t="s">
+        <v>106</v>
+      </c>
+      <c r="F27" s="7">
+        <v>32524</v>
+      </c>
+      <c r="G27" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="H27" s="2">
+        <v>723.3</v>
+      </c>
+      <c r="I27" s="2">
+        <v>601.74</v>
+      </c>
+      <c r="J27" s="2">
+        <v>79.69</v>
+      </c>
+      <c r="K27" s="2">
+        <v>30.09</v>
+      </c>
+      <c r="L27" t="s">
+        <v>29</v>
+      </c>
+      <c r="M27" t="s">
+        <v>16</v>
+      </c>
+      <c r="N27" s="2">
+        <v>5</v>
+      </c>
+      <c r="O27" s="2">
+        <v>2025</v>
+      </c>
+    </row>
+    <row r="28" spans="1:15" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A28" t="s">
+        <v>103</v>
+      </c>
+      <c r="B28" t="s">
+        <v>104</v>
+      </c>
+      <c r="C28" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D28" t="s">
+        <v>105</v>
+      </c>
+      <c r="E28" t="s">
+        <v>106</v>
+      </c>
+      <c r="F28" s="7">
+        <v>32524</v>
+      </c>
+      <c r="G28" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="H28" s="2">
+        <v>4307.1899999999996</v>
+      </c>
+      <c r="I28" s="2">
+        <v>3585.72</v>
+      </c>
+      <c r="J28" s="2">
+        <v>474.92</v>
+      </c>
+      <c r="K28" s="2">
+        <v>179.29</v>
+      </c>
+      <c r="L28" t="s">
+        <v>112</v>
+      </c>
+      <c r="M28" t="s">
+        <v>113</v>
+      </c>
+      <c r="N28" s="2">
+        <v>5</v>
+      </c>
+      <c r="O28" s="2">
+        <v>2025</v>
+      </c>
+    </row>
+    <row r="29" spans="1:15" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A29" t="s">
+        <v>103</v>
+      </c>
+      <c r="B29" t="s">
+        <v>104</v>
+      </c>
+      <c r="C29" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D29" t="s">
+        <v>105</v>
+      </c>
+      <c r="E29" t="s">
+        <v>106</v>
+      </c>
+      <c r="F29" s="7">
+        <v>32524</v>
+      </c>
+      <c r="G29" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="H29" s="2">
+        <v>1446.63</v>
+      </c>
+      <c r="I29" s="2">
+        <v>1203.48</v>
+      </c>
+      <c r="J29" s="2">
+        <v>159.38</v>
+      </c>
+      <c r="K29" s="2">
+        <v>60.17</v>
+      </c>
+      <c r="L29" t="s">
+        <v>112</v>
+      </c>
+      <c r="M29" t="s">
+        <v>113</v>
+      </c>
+      <c r="N29" s="2">
+        <v>5</v>
+      </c>
+      <c r="O29" s="2">
+        <v>2025</v>
+      </c>
+    </row>
+    <row r="30" spans="1:15" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A30" t="s">
+        <v>103</v>
+      </c>
+      <c r="B30" t="s">
+        <v>104</v>
+      </c>
+      <c r="C30" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D30" t="s">
+        <v>105</v>
+      </c>
+      <c r="E30" t="s">
+        <v>106</v>
+      </c>
+      <c r="F30" s="7">
+        <v>32524</v>
+      </c>
+      <c r="G30" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="H30" s="2">
+        <v>1800.36</v>
+      </c>
+      <c r="I30" s="2">
+        <v>1504.35</v>
+      </c>
+      <c r="J30" s="2">
+        <v>198.15</v>
+      </c>
+      <c r="K30" s="2">
+        <v>75.22</v>
+      </c>
+      <c r="L30" t="s">
+        <v>29</v>
+      </c>
+      <c r="M30" t="s">
+        <v>16</v>
+      </c>
+      <c r="N30" s="2">
+        <v>5</v>
+      </c>
+      <c r="O30" s="2">
+        <v>2025</v>
+      </c>
+    </row>
+    <row r="31" spans="1:15" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A31" t="s">
+        <v>103</v>
+      </c>
+      <c r="B31" t="s">
+        <v>104</v>
+      </c>
+      <c r="C31" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D31" t="s">
+        <v>105</v>
+      </c>
+      <c r="E31" t="s">
+        <v>106</v>
+      </c>
+      <c r="F31" s="7">
+        <v>32524</v>
+      </c>
+      <c r="G31" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="H31" s="2">
+        <v>1440.32</v>
+      </c>
+      <c r="I31" s="2">
+        <v>1203.48</v>
+      </c>
+      <c r="J31" s="2">
+        <v>158.52000000000001</v>
+      </c>
+      <c r="K31" s="2">
+        <v>60.17</v>
+      </c>
+      <c r="L31" t="s">
+        <v>112</v>
+      </c>
+      <c r="M31" t="s">
+        <v>113</v>
+      </c>
+      <c r="N31" s="2">
+        <v>5</v>
+      </c>
+      <c r="O31" s="2">
+        <v>2025</v>
+      </c>
+    </row>
+    <row r="32" spans="1:15" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A32" t="s">
+        <v>117</v>
+      </c>
+      <c r="B32" t="s">
+        <v>118</v>
+      </c>
+      <c r="C32" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D32" t="s">
+        <v>119</v>
+      </c>
+      <c r="E32" t="s">
+        <v>120</v>
+      </c>
+      <c r="F32" s="7">
+        <v>32770</v>
+      </c>
+      <c r="G32" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="H32" s="2">
+        <v>7730.97</v>
+      </c>
+      <c r="I32" s="2">
+        <v>7530.2</v>
+      </c>
+      <c r="J32" s="2">
+        <v>994.51</v>
+      </c>
+      <c r="K32" s="2">
+        <v>376.51</v>
+      </c>
+      <c r="L32" t="s">
+        <v>15</v>
+      </c>
+      <c r="M32" t="s">
+        <v>30</v>
+      </c>
+      <c r="N32" s="2">
+        <v>5</v>
+      </c>
+      <c r="O32" s="2">
+        <v>2025</v>
+      </c>
+    </row>
+    <row r="33" spans="1:15" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A33" t="s">
+        <v>122</v>
+      </c>
+      <c r="B33" t="s">
+        <v>123</v>
+      </c>
+      <c r="C33" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="D33" t="s">
+        <v>124</v>
+      </c>
+      <c r="E33" t="s">
+        <v>125</v>
+      </c>
+      <c r="F33" s="7">
+        <v>32419</v>
+      </c>
+      <c r="G33" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="H33" s="2">
+        <v>19596.099999999999</v>
+      </c>
+      <c r="I33" s="2">
+        <v>17635.04</v>
+      </c>
+      <c r="J33" s="2">
+        <v>2333.8200000000002</v>
+      </c>
+      <c r="K33" s="2">
+        <v>881.75</v>
+      </c>
+      <c r="L33" t="s">
+        <v>71</v>
+      </c>
+      <c r="M33" t="s">
+        <v>113</v>
+      </c>
+      <c r="N33" s="2">
+        <v>5</v>
+      </c>
+      <c r="O33" s="2">
+        <v>2025</v>
+      </c>
+    </row>
+    <row r="34" spans="1:15" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A34" t="s">
+        <v>127</v>
+      </c>
+      <c r="B34" t="s">
+        <v>128</v>
+      </c>
+      <c r="C34" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D34" t="s">
+        <v>129</v>
+      </c>
+      <c r="E34" t="s">
+        <v>130</v>
+      </c>
+      <c r="F34" s="7">
+        <v>32225</v>
+      </c>
+      <c r="G34" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="H34" s="2">
+        <v>772.52</v>
+      </c>
+      <c r="I34" s="2">
+        <v>601.74</v>
+      </c>
+      <c r="J34" s="2">
+        <v>79.69</v>
+      </c>
+      <c r="K34" s="2">
+        <v>30.09</v>
+      </c>
+      <c r="L34" t="s">
+        <v>132</v>
+      </c>
+      <c r="M34" t="s">
+        <v>30</v>
+      </c>
+      <c r="N34" s="2">
+        <v>5</v>
+      </c>
+      <c r="O34" s="2">
+        <v>2025</v>
+      </c>
+    </row>
+    <row r="35" spans="1:15" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A35" t="s">
+        <v>127</v>
+      </c>
+      <c r="B35" t="s">
+        <v>128</v>
+      </c>
+      <c r="C35" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D35" t="s">
+        <v>129</v>
+      </c>
+      <c r="E35" t="s">
+        <v>130</v>
+      </c>
+      <c r="F35" s="7">
+        <v>32225</v>
+      </c>
+      <c r="G35" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="H35" s="2">
+        <v>386.25</v>
+      </c>
+      <c r="I35" s="2">
+        <v>300.87</v>
+      </c>
+      <c r="J35" s="2">
+        <v>39.840000000000003</v>
+      </c>
+      <c r="K35" s="2">
+        <v>15.04</v>
+      </c>
+      <c r="L35" t="s">
+        <v>132</v>
+      </c>
+      <c r="M35" t="s">
+        <v>30</v>
+      </c>
+      <c r="N35" s="2">
+        <v>5</v>
+      </c>
+      <c r="O35" s="2">
+        <v>2025</v>
+      </c>
+    </row>
+    <row r="36" spans="1:15" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A36" t="s">
+        <v>127</v>
+      </c>
+      <c r="B36" t="s">
+        <v>128</v>
+      </c>
+      <c r="C36" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D36" t="s">
+        <v>129</v>
+      </c>
+      <c r="E36" t="s">
+        <v>130</v>
+      </c>
+      <c r="F36" s="7">
+        <v>32225</v>
+      </c>
+      <c r="G36" s="2" t="s">
+        <v>134</v>
+      </c>
+      <c r="H36" s="2">
+        <v>1931.28</v>
+      </c>
+      <c r="I36" s="2">
+        <v>1504.35</v>
+      </c>
+      <c r="J36" s="2">
+        <v>199.22</v>
+      </c>
+      <c r="K36" s="2">
+        <v>75.22</v>
+      </c>
+      <c r="L36" t="s">
+        <v>132</v>
+      </c>
+      <c r="M36" t="s">
+        <v>30</v>
+      </c>
+      <c r="N36" s="2">
+        <v>5</v>
+      </c>
+      <c r="O36" s="2">
+        <v>2025</v>
+      </c>
+    </row>
+    <row r="37" spans="1:15" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A37" t="s">
+        <v>127</v>
+      </c>
+      <c r="B37" t="s">
+        <v>128</v>
+      </c>
+      <c r="C37" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D37" t="s">
+        <v>129</v>
+      </c>
+      <c r="E37" t="s">
+        <v>130</v>
+      </c>
+      <c r="F37" s="7">
+        <v>32225</v>
+      </c>
+      <c r="G37" s="2" t="s">
+        <v>135</v>
+      </c>
+      <c r="H37" s="2">
+        <v>1931.28</v>
+      </c>
+      <c r="I37" s="2">
+        <v>1504.35</v>
+      </c>
+      <c r="J37" s="2">
+        <v>199.22</v>
+      </c>
+      <c r="K37" s="2">
+        <v>75.22</v>
+      </c>
+      <c r="L37" t="s">
+        <v>132</v>
+      </c>
+      <c r="M37" t="s">
+        <v>30</v>
+      </c>
+      <c r="N37" s="2">
+        <v>5</v>
+      </c>
+      <c r="O37" s="2">
+        <v>2025</v>
+      </c>
+    </row>
+    <row r="38" spans="1:15" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A38" t="s">
+        <v>127</v>
+      </c>
+      <c r="B38" t="s">
+        <v>128</v>
+      </c>
+      <c r="C38" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D38" t="s">
+        <v>129</v>
+      </c>
+      <c r="E38" t="s">
+        <v>130</v>
+      </c>
+      <c r="F38" s="7">
+        <v>32225</v>
+      </c>
+      <c r="G38" s="2" t="s">
+        <v>136</v>
+      </c>
+      <c r="H38" s="2">
+        <v>772.52</v>
+      </c>
+      <c r="I38" s="2">
+        <v>601.74</v>
+      </c>
+      <c r="J38" s="2">
+        <v>79.69</v>
+      </c>
+      <c r="K38" s="2">
+        <v>30.09</v>
+      </c>
+      <c r="L38" t="s">
+        <v>132</v>
+      </c>
+      <c r="M38" t="s">
+        <v>30</v>
+      </c>
+      <c r="N38" s="2">
+        <v>5</v>
+      </c>
+      <c r="O38" s="2">
+        <v>2025</v>
+      </c>
+    </row>
+    <row r="39" spans="1:15" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A39" t="s">
+        <v>127</v>
+      </c>
+      <c r="B39" t="s">
+        <v>128</v>
+      </c>
+      <c r="C39" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D39" t="s">
+        <v>129</v>
+      </c>
+      <c r="E39" t="s">
+        <v>130</v>
+      </c>
+      <c r="F39" s="7">
+        <v>32225</v>
+      </c>
+      <c r="G39" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="H39" s="2">
+        <v>3827.56</v>
+      </c>
+      <c r="I39" s="2">
+        <v>3008.7</v>
+      </c>
+      <c r="J39" s="2">
+        <v>398.44</v>
+      </c>
+      <c r="K39" s="2">
+        <v>150.44</v>
+      </c>
+      <c r="L39" t="s">
+        <v>132</v>
+      </c>
+      <c r="M39" t="s">
+        <v>30</v>
+      </c>
+      <c r="N39" s="2">
+        <v>5</v>
+      </c>
+      <c r="O39" s="2">
+        <v>2025</v>
+      </c>
+    </row>
+    <row r="40" spans="1:15" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A40" t="s">
+        <v>127</v>
+      </c>
+      <c r="B40" t="s">
+        <v>128</v>
+      </c>
+      <c r="C40" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D40" t="s">
+        <v>129</v>
+      </c>
+      <c r="E40" t="s">
+        <v>130</v>
+      </c>
+      <c r="F40" s="7">
+        <v>32225</v>
+      </c>
+      <c r="G40" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="H40" s="2">
+        <v>1783.72</v>
+      </c>
+      <c r="I40" s="2">
+        <v>1504.35</v>
+      </c>
+      <c r="J40" s="2">
+        <v>199.22</v>
+      </c>
+      <c r="K40" s="2">
+        <v>75.22</v>
+      </c>
+      <c r="L40" t="s">
+        <v>132</v>
+      </c>
+      <c r="M40" t="s">
+        <v>30</v>
+      </c>
+      <c r="N40" s="2">
+        <v>5</v>
+      </c>
+      <c r="O40" s="2">
+        <v>2025</v>
+      </c>
+    </row>
+    <row r="41" spans="1:15" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A41" t="s">
+        <v>139</v>
+      </c>
+      <c r="B41" t="s">
+        <v>140</v>
+      </c>
+      <c r="C41" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D41" t="s">
+        <v>141</v>
+      </c>
+      <c r="E41" t="s">
+        <v>142</v>
+      </c>
+      <c r="F41" s="7">
+        <v>32755</v>
+      </c>
+      <c r="G41" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="H41" s="2">
+        <v>9857.1299999999992</v>
+      </c>
+      <c r="I41" s="2">
+        <v>8424.36</v>
+      </c>
+      <c r="J41" s="2">
+        <v>1119.02</v>
+      </c>
+      <c r="K41" s="2">
+        <v>421.22</v>
+      </c>
+      <c r="L41" t="s">
+        <v>36</v>
+      </c>
+      <c r="M41" t="s">
+        <v>16</v>
+      </c>
+      <c r="N41" s="2">
+        <v>5</v>
+      </c>
+      <c r="O41" s="2">
+        <v>2025</v>
+      </c>
+    </row>
+    <row r="42" spans="1:15" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A42" t="s">
+        <v>139</v>
+      </c>
+      <c r="B42" t="s">
+        <v>140</v>
+      </c>
+      <c r="C42" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D42" t="s">
+        <v>141</v>
+      </c>
+      <c r="E42" t="s">
+        <v>142</v>
+      </c>
+      <c r="F42" s="7">
+        <v>32755</v>
+      </c>
+      <c r="G42" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="H42" s="2">
+        <v>1373.18</v>
+      </c>
+      <c r="I42" s="2">
+        <v>1203.48</v>
+      </c>
+      <c r="J42" s="2">
+        <v>159.86000000000001</v>
+      </c>
+      <c r="K42" s="2">
+        <v>60.17</v>
+      </c>
+      <c r="L42" t="s">
+        <v>36</v>
+      </c>
+      <c r="M42" t="s">
+        <v>16</v>
+      </c>
+      <c r="N42" s="2">
+        <v>5</v>
+      </c>
+      <c r="O42" s="2">
+        <v>2025</v>
+      </c>
+    </row>
+    <row r="43" spans="1:15" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A43" t="s">
+        <v>139</v>
+      </c>
+      <c r="B43" t="s">
+        <v>140</v>
+      </c>
+      <c r="C43" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D43" t="s">
+        <v>141</v>
+      </c>
+      <c r="E43" t="s">
+        <v>142</v>
+      </c>
+      <c r="F43" s="7">
+        <v>32755</v>
+      </c>
+      <c r="G43" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="H43" s="2">
+        <v>1760.2</v>
+      </c>
+      <c r="I43" s="2">
+        <v>1504.35</v>
+      </c>
+      <c r="J43" s="2">
+        <v>199.82</v>
+      </c>
+      <c r="K43" s="2">
+        <v>75.22</v>
+      </c>
+      <c r="L43" t="s">
+        <v>36</v>
+      </c>
+      <c r="M43" t="s">
+        <v>16</v>
+      </c>
+      <c r="N43" s="2">
+        <v>5</v>
+      </c>
+      <c r="O43" s="2">
+        <v>2025</v>
+      </c>
+    </row>
+    <row r="44" spans="1:15" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A44" t="s">
+        <v>146</v>
+      </c>
+      <c r="B44" t="s">
+        <v>147</v>
+      </c>
+      <c r="C44" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="D44" t="s">
+        <v>148</v>
+      </c>
+      <c r="E44" t="s">
+        <v>149</v>
+      </c>
+      <c r="F44" s="7">
+        <v>32510</v>
+      </c>
+      <c r="G44" s="2" t="s">
+        <v>150</v>
+      </c>
+      <c r="H44" s="2">
+        <v>23459.48</v>
+      </c>
+      <c r="I44" s="2">
+        <v>17279.75</v>
+      </c>
+      <c r="J44" s="2">
+        <v>2684.83</v>
+      </c>
+      <c r="K44" s="2">
+        <v>863.99</v>
+      </c>
+      <c r="L44" t="s">
+        <v>36</v>
+      </c>
+      <c r="M44" t="s">
+        <v>16</v>
+      </c>
+      <c r="N44" s="2">
+        <v>5</v>
+      </c>
+      <c r="O44" s="2">
+        <v>2025</v>
+      </c>
+    </row>
+    <row r="45" spans="1:15" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A45" t="s">
+        <v>151</v>
+      </c>
+      <c r="B45" t="s">
+        <v>152</v>
+      </c>
+      <c r="C45" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="D45" t="s">
+        <v>153</v>
+      </c>
+      <c r="E45" t="s">
+        <v>154</v>
+      </c>
+      <c r="F45" s="7">
+        <v>32758</v>
+      </c>
+      <c r="G45" s="2" t="s">
+        <v>155</v>
+      </c>
+      <c r="H45" s="2">
+        <v>16748.71</v>
+      </c>
+      <c r="I45" s="2">
+        <v>7780.34</v>
+      </c>
+      <c r="J45" s="2">
+        <v>1028.33</v>
+      </c>
+      <c r="K45" s="2">
+        <v>389.02</v>
+      </c>
+      <c r="L45" t="s">
+        <v>36</v>
+      </c>
+      <c r="M45" t="s">
+        <v>16</v>
+      </c>
+      <c r="N45" s="2">
+        <v>5</v>
+      </c>
+      <c r="O45" s="2">
+        <v>2025</v>
+      </c>
+    </row>
+    <row r="46" spans="1:15" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A46" t="s">
+        <v>156</v>
+      </c>
+      <c r="B46" t="s">
+        <v>157</v>
+      </c>
+      <c r="C46" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="D46" t="s">
+        <v>158</v>
+      </c>
+      <c r="E46" t="s">
+        <v>159</v>
+      </c>
+      <c r="F46" s="7">
+        <v>32752</v>
+      </c>
+      <c r="G46" s="2" t="s">
+        <v>160</v>
+      </c>
+      <c r="H46" s="2">
+        <v>7160.79</v>
+      </c>
+      <c r="I46" s="2">
+        <v>4542.0200000000004</v>
+      </c>
+      <c r="J46" s="2">
+        <v>586.05999999999995</v>
+      </c>
+      <c r="K46" s="2">
+        <v>227.1</v>
+      </c>
+      <c r="L46" t="s">
+        <v>161</v>
+      </c>
+      <c r="M46" t="s">
+        <v>16</v>
+      </c>
+      <c r="N46" s="2">
+        <v>5</v>
+      </c>
+      <c r="O46" s="2">
+        <v>2025</v>
+      </c>
+    </row>
+    <row r="47" spans="1:15" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A47" t="s">
+        <v>162</v>
+      </c>
+      <c r="B47" t="s">
+        <v>163</v>
+      </c>
+      <c r="C47" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D47" t="s">
+        <v>164</v>
+      </c>
+      <c r="E47" t="s">
+        <v>165</v>
+      </c>
+      <c r="F47" s="7">
+        <v>32783</v>
+      </c>
+      <c r="G47" s="2" t="s">
+        <v>166</v>
+      </c>
+      <c r="H47" s="2">
+        <v>9218.31</v>
+      </c>
+      <c r="I47" s="2">
+        <v>5900.12</v>
+      </c>
+      <c r="J47" s="2">
+        <v>780.61</v>
+      </c>
+      <c r="K47" s="2">
+        <v>295.01</v>
+      </c>
+      <c r="L47" t="s">
+        <v>36</v>
+      </c>
+      <c r="M47" t="s">
+        <v>113</v>
+      </c>
+      <c r="N47" s="2">
+        <v>5</v>
+      </c>
+      <c r="O47" s="2">
+        <v>2025</v>
+      </c>
+    </row>
+    <row r="48" spans="1:15" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A48" t="s">
+        <v>167</v>
+      </c>
+      <c r="B48" t="s">
+        <v>168</v>
+      </c>
+      <c r="C48" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="D48" t="s">
+        <v>169</v>
+      </c>
+      <c r="E48" t="s">
+        <v>170</v>
+      </c>
+      <c r="F48" s="7">
+        <v>32752</v>
+      </c>
+      <c r="G48" s="2" t="s">
+        <v>171</v>
+      </c>
+      <c r="H48" s="2">
+        <v>26592.71</v>
+      </c>
+      <c r="I48" s="2">
+        <v>17635.04</v>
+      </c>
+      <c r="J48" s="2">
+        <v>2724.36</v>
+      </c>
+      <c r="K48" s="2">
+        <v>881.75</v>
+      </c>
+      <c r="L48" t="s">
+        <v>172</v>
+      </c>
+      <c r="M48" t="s">
+        <v>16</v>
+      </c>
+      <c r="N48" s="2">
+        <v>5</v>
+      </c>
+      <c r="O48" s="2">
         <v>2025</v>
       </c>
     </row>

</xml_diff>